<commit_message>
Some small formatting changes
</commit_message>
<xml_diff>
--- a/Literature Overview.xlsx
+++ b/Literature Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a2b252fdecbd1de8/Studie/Master Forensic Science/Literature Thesis/CllrLiteratureThesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2409" documentId="13_ncr:1_{234FEDD6-FF7B-B74F-9E91-30AF20864B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{165AABCD-B16F-A342-9C22-591875E4699D}"/>
+  <xr:revisionPtr revIDLastSave="2411" documentId="13_ncr:1_{234FEDD6-FF7B-B74F-9E91-30AF20864B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3AC0E26-568F-4DD5-8955-005AF2BB51B5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{66F3E14A-ACD8-714D-B4C4-32841F231FE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{66F3E14A-ACD8-714D-B4C4-32841F231FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="869">
   <si>
     <t>Year</t>
   </si>
@@ -2439,9 +2443,6 @@
   </si>
   <si>
     <t>False - Too small sample for proper validation</t>
-  </si>
-  <si>
-    <t>True - Calculated</t>
   </si>
   <si>
     <t>Germany/Italy/India/Australia/Netherlands (NFI)/Switzerland</t>
@@ -3094,32 +3095,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520F41DF-5CC0-8644-B142-924A5334297A}">
   <dimension ref="A1:W176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G136" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O172" sqref="O172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" customWidth="1"/>
-    <col min="4" max="4" width="73.1640625" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" customWidth="1"/>
-    <col min="6" max="7" width="26.1640625" customWidth="1"/>
-    <col min="8" max="8" width="44.83203125" customWidth="1"/>
-    <col min="9" max="11" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.875" customWidth="1"/>
+    <col min="3" max="3" width="39.625" customWidth="1"/>
+    <col min="4" max="4" width="73.125" customWidth="1"/>
+    <col min="5" max="5" width="36.625" customWidth="1"/>
+    <col min="6" max="7" width="26.125" customWidth="1"/>
+    <col min="8" max="8" width="44.875" customWidth="1"/>
+    <col min="9" max="11" width="26.125" customWidth="1"/>
     <col min="12" max="14" width="34" customWidth="1"/>
     <col min="15" max="15" width="72" customWidth="1"/>
-    <col min="16" max="16" width="119.33203125" customWidth="1"/>
-    <col min="17" max="17" width="105.6640625" customWidth="1"/>
+    <col min="16" max="16" width="119.375" customWidth="1"/>
+    <col min="17" max="17" width="105.625" customWidth="1"/>
     <col min="18" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="45.33203125" customWidth="1"/>
-    <col min="21" max="21" width="59.1640625" customWidth="1"/>
-    <col min="22" max="22" width="88.1640625" customWidth="1"/>
-    <col min="23" max="23" width="33.6640625" customWidth="1"/>
+    <col min="20" max="20" width="45.375" customWidth="1"/>
+    <col min="21" max="21" width="59.125" customWidth="1"/>
+    <col min="22" max="22" width="88.125" customWidth="1"/>
+    <col min="23" max="23" width="33.625" customWidth="1"/>
     <col min="24" max="24" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3127,10 +3128,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -3190,7 +3191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2006</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>756</v>
       </c>
       <c r="C2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D2" t="s">
         <v>771</v>
@@ -3247,7 +3248,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2007</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>552</v>
       </c>
       <c r="C4" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D4" t="s">
         <v>776</v>
@@ -3311,7 +3312,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2007</v>
       </c>
@@ -3319,7 +3320,7 @@
         <v>568</v>
       </c>
       <c r="C5" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D5" t="s">
         <v>775</v>
@@ -3343,7 +3344,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2007</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>572</v>
       </c>
       <c r="C6" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D6" t="s">
         <v>774</v>
@@ -3375,7 +3376,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>589</v>
       </c>
       <c r="C7" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D7" t="s">
         <v>773</v>
@@ -3407,7 +3408,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2009</v>
       </c>
@@ -3439,7 +3440,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -3512,10 +3513,10 @@
         <v>620</v>
       </c>
       <c r="C10" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D10" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E10" t="s">
         <v>621</v>
@@ -3536,7 +3537,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -3595,7 +3596,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -3654,7 +3655,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -3662,7 +3663,7 @@
         <v>290</v>
       </c>
       <c r="C13" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D13" t="s">
         <v>781</v>
@@ -3711,7 +3712,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -3719,7 +3720,7 @@
         <v>511</v>
       </c>
       <c r="C14" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D14" t="s">
         <v>782</v>
@@ -3767,7 +3768,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -3775,7 +3776,7 @@
         <v>511</v>
       </c>
       <c r="C15" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D15" t="s">
         <v>782</v>
@@ -3823,7 +3824,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>511</v>
       </c>
       <c r="C16" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D16" t="s">
         <v>782</v>
@@ -3879,7 +3880,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2011</v>
       </c>
@@ -3887,7 +3888,7 @@
         <v>511</v>
       </c>
       <c r="C17" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D17" t="s">
         <v>782</v>
@@ -3935,7 +3936,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -3970,7 +3971,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2011</v>
       </c>
@@ -4002,7 +4003,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2011</v>
       </c>
@@ -4010,7 +4011,7 @@
         <v>615</v>
       </c>
       <c r="C20" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D20" t="s">
         <v>785</v>
@@ -4034,7 +4035,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2011</v>
       </c>
@@ -4097,7 +4098,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2012</v>
       </c>
@@ -4129,7 +4130,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2012</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>617</v>
       </c>
       <c r="C23" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D23" t="s">
         <v>774</v>
@@ -4161,7 +4162,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2012</v>
       </c>
@@ -4199,7 +4200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2013</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2013</v>
       </c>
@@ -4305,7 +4306,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2013</v>
       </c>
@@ -4358,7 +4359,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2013</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2013</v>
       </c>
@@ -4422,7 +4423,7 @@
         <v>757</v>
       </c>
       <c r="C29" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D29" t="s">
         <v>790</v>
@@ -4470,7 +4471,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2013</v>
       </c>
@@ -4524,7 +4525,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2013</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2013</v>
       </c>
@@ -4642,7 +4643,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2013</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>759</v>
       </c>
       <c r="C33" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D33" t="s">
         <v>774</v>
@@ -4680,7 +4681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2014</v>
       </c>
@@ -4688,7 +4689,7 @@
         <v>356</v>
       </c>
       <c r="C34" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D34" t="s">
         <v>779</v>
@@ -4739,7 +4740,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2014</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>261</v>
       </c>
       <c r="C35" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D35" t="s">
         <v>793</v>
@@ -4802,7 +4803,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -4810,7 +4811,7 @@
         <v>235</v>
       </c>
       <c r="C36" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D36" t="s">
         <v>794</v>
@@ -4862,7 +4863,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2014</v>
       </c>
@@ -4918,7 +4919,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2014</v>
       </c>
@@ -4974,7 +4975,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2014</v>
       </c>
@@ -4982,7 +4983,7 @@
         <v>548</v>
       </c>
       <c r="C39" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D39" t="s">
         <v>774</v>
@@ -5006,7 +5007,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2014</v>
       </c>
@@ -5014,7 +5015,7 @@
         <v>576</v>
       </c>
       <c r="C40" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D40" t="s">
         <v>779</v>
@@ -5038,7 +5039,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2014</v>
       </c>
@@ -5046,10 +5047,10 @@
         <v>696</v>
       </c>
       <c r="C41" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D41" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E41" t="s">
         <v>697</v>
@@ -5073,7 +5074,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2015</v>
       </c>
@@ -5081,10 +5082,10 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D42" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E42" t="s">
         <v>40</v>
@@ -5132,7 +5133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2015</v>
       </c>
@@ -5191,7 +5192,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2015</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2015</v>
       </c>
@@ -5311,7 +5312,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2015</v>
       </c>
@@ -5371,7 +5372,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2015</v>
       </c>
@@ -5424,7 +5425,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2015</v>
       </c>
@@ -5480,7 +5481,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2015</v>
       </c>
@@ -5539,7 +5540,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2015</v>
       </c>
@@ -5601,7 +5602,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2015</v>
       </c>
@@ -5609,10 +5610,10 @@
         <v>437</v>
       </c>
       <c r="C51" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D51" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E51" t="s">
         <v>438</v>
@@ -5667,7 +5668,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2015</v>
       </c>
@@ -5675,10 +5676,10 @@
         <v>362</v>
       </c>
       <c r="C52" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D52" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E52" t="s">
         <v>363</v>
@@ -5720,7 +5721,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2015</v>
       </c>
@@ -5728,10 +5729,10 @@
         <v>437</v>
       </c>
       <c r="C53" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D53" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E53" t="s">
         <v>438</v>
@@ -5786,7 +5787,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2015</v>
       </c>
@@ -5794,10 +5795,10 @@
         <v>437</v>
       </c>
       <c r="C54" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D54" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E54" t="s">
         <v>438</v>
@@ -5852,7 +5853,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2015</v>
       </c>
@@ -5860,10 +5861,10 @@
         <v>584</v>
       </c>
       <c r="C55" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D55" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E55" t="s">
         <v>585</v>
@@ -5884,7 +5885,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2016</v>
       </c>
@@ -5940,7 +5941,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2016</v>
       </c>
@@ -5999,7 +6000,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2016</v>
       </c>
@@ -6055,7 +6056,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2016</v>
       </c>
@@ -6118,7 +6119,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2016</v>
       </c>
@@ -6126,7 +6127,7 @@
         <v>210</v>
       </c>
       <c r="C60" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D60" t="s">
         <v>779</v>
@@ -6171,7 +6172,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2016</v>
       </c>
@@ -6230,7 +6231,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2016</v>
       </c>
@@ -6238,10 +6239,10 @@
         <v>313</v>
       </c>
       <c r="C62" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D62" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E62" t="s">
         <v>314</v>
@@ -6292,7 +6293,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2016</v>
       </c>
@@ -6349,7 +6350,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2016</v>
       </c>
@@ -6408,7 +6409,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2016</v>
       </c>
@@ -6416,10 +6417,10 @@
         <v>184</v>
       </c>
       <c r="C65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E65" t="s">
         <v>185</v>
@@ -6464,7 +6465,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2016</v>
       </c>
@@ -6502,7 +6503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2016</v>
       </c>
@@ -6510,10 +6511,10 @@
         <v>709</v>
       </c>
       <c r="C67" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D67" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E67" t="s">
         <v>710</v>
@@ -6534,7 +6535,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2017</v>
       </c>
@@ -6542,10 +6543,10 @@
         <v>99</v>
       </c>
       <c r="C68" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D68" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E68" t="s">
         <v>100</v>
@@ -6596,7 +6597,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2017</v>
       </c>
@@ -6655,7 +6656,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2017</v>
       </c>
@@ -6714,7 +6715,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2017</v>
       </c>
@@ -6770,7 +6771,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2017</v>
       </c>
@@ -6778,10 +6779,10 @@
         <v>191</v>
       </c>
       <c r="C72" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D72" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E72" t="s">
         <v>192</v>
@@ -6826,7 +6827,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2017</v>
       </c>
@@ -6834,10 +6835,10 @@
         <v>273</v>
       </c>
       <c r="C73" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D73" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E73" t="s">
         <v>274</v>
@@ -6885,7 +6886,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2017</v>
       </c>
@@ -6893,10 +6894,10 @@
         <v>214</v>
       </c>
       <c r="C74" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D74" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E74" t="s">
         <v>215</v>
@@ -6944,7 +6945,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2017</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2017</v>
       </c>
@@ -7062,7 +7063,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2017</v>
       </c>
@@ -7118,7 +7119,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2017</v>
       </c>
@@ -7184,7 +7185,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2017</v>
       </c>
@@ -7192,10 +7193,10 @@
         <v>558</v>
       </c>
       <c r="C79" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D79" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E79" t="s">
         <v>559</v>
@@ -7216,7 +7217,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2017</v>
       </c>
@@ -7224,7 +7225,7 @@
         <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D80" t="s">
         <v>779</v>
@@ -7279,7 +7280,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2018</v>
       </c>
@@ -7287,10 +7288,10 @@
         <v>765</v>
       </c>
       <c r="C81" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D81" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E81" t="s">
         <v>306</v>
@@ -7342,7 +7343,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2018</v>
       </c>
@@ -7395,7 +7396,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2018</v>
       </c>
@@ -7403,10 +7404,10 @@
         <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D83" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E83" t="s">
         <v>96</v>
@@ -7451,7 +7452,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2018</v>
       </c>
@@ -7504,7 +7505,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2018</v>
       </c>
@@ -7560,7 +7561,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2018</v>
       </c>
@@ -7568,10 +7569,10 @@
         <v>118</v>
       </c>
       <c r="C86" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D86" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E86" t="s">
         <v>119</v>
@@ -7619,7 +7620,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2018</v>
       </c>
@@ -7627,10 +7628,10 @@
         <v>118</v>
       </c>
       <c r="C87" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D87" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E87" t="s">
         <v>406</v>
@@ -7684,7 +7685,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2018</v>
       </c>
@@ -7692,10 +7693,10 @@
         <v>248</v>
       </c>
       <c r="C88" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D88" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E88" t="s">
         <v>249</v>
@@ -7740,7 +7741,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2018</v>
       </c>
@@ -7802,7 +7803,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2018</v>
       </c>
@@ -7861,7 +7862,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2018</v>
       </c>
@@ -7896,7 +7897,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2019</v>
       </c>
@@ -7904,10 +7905,10 @@
         <v>388</v>
       </c>
       <c r="C92" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D92" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E92" t="s">
         <v>389</v>
@@ -7956,7 +7957,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2019</v>
       </c>
@@ -7964,10 +7965,10 @@
         <v>219</v>
       </c>
       <c r="C93" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D93" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E93" t="s">
         <v>225</v>
@@ -8018,7 +8019,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2019</v>
       </c>
@@ -8026,10 +8027,10 @@
         <v>230</v>
       </c>
       <c r="C94" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D94" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E94" t="s">
         <v>231</v>
@@ -8077,7 +8078,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2019</v>
       </c>
@@ -8085,10 +8086,10 @@
         <v>219</v>
       </c>
       <c r="C95" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D95" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E95" t="s">
         <v>220</v>
@@ -8139,7 +8140,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2019</v>
       </c>
@@ -8171,7 +8172,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2019</v>
       </c>
@@ -8179,10 +8180,10 @@
         <v>368</v>
       </c>
       <c r="C97" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D97" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E97" t="s">
         <v>369</v>
@@ -8227,7 +8228,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2019</v>
       </c>
@@ -8283,7 +8284,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2019</v>
       </c>
@@ -8339,7 +8340,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2019</v>
       </c>
@@ -8374,7 +8375,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2019</v>
       </c>
@@ -8382,10 +8383,10 @@
         <v>545</v>
       </c>
       <c r="C101" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D101" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E101" t="s">
         <v>546</v>
@@ -8406,7 +8407,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2019</v>
       </c>
@@ -8414,7 +8415,7 @@
         <v>560</v>
       </c>
       <c r="C102" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D102" t="s">
         <v>779</v>
@@ -8438,7 +8439,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2019</v>
       </c>
@@ -8446,13 +8447,13 @@
         <v>665</v>
       </c>
       <c r="C103" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D103" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E103" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G103" t="s">
         <v>173</v>
@@ -8470,7 +8471,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2019</v>
       </c>
@@ -8505,7 +8506,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2019</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2019</v>
       </c>
@@ -8545,7 +8546,7 @@
         <v>560</v>
       </c>
       <c r="C106" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D106" t="s">
         <v>779</v>
@@ -8572,7 +8573,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2019</v>
       </c>
@@ -8580,10 +8581,10 @@
         <v>701</v>
       </c>
       <c r="C107" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D107" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E107" t="s">
         <v>702</v>
@@ -8607,7 +8608,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2019</v>
       </c>
@@ -8615,10 +8616,10 @@
         <v>704</v>
       </c>
       <c r="C108" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D108" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E108" t="s">
         <v>705</v>
@@ -8642,7 +8643,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2019</v>
       </c>
@@ -8650,10 +8651,10 @@
         <v>707</v>
       </c>
       <c r="C109" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D109" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E109" t="s">
         <v>708</v>
@@ -8674,7 +8675,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2019</v>
       </c>
@@ -8682,10 +8683,10 @@
         <v>713</v>
       </c>
       <c r="C110" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D110" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E110" t="s">
         <v>714</v>
@@ -8719,7 +8720,7 @@
         <v>161</v>
       </c>
       <c r="O110" t="s">
-        <v>802</v>
+        <v>725</v>
       </c>
       <c r="P110" t="s">
         <v>44</v>
@@ -8734,7 +8735,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2020</v>
       </c>
@@ -8742,10 +8743,10 @@
         <v>466</v>
       </c>
       <c r="C111" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D111" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E111" t="s">
         <v>467</v>
@@ -8790,7 +8791,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2020</v>
       </c>
@@ -8840,7 +8841,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2020</v>
       </c>
@@ -8848,10 +8849,10 @@
         <v>50</v>
       </c>
       <c r="C113" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D113" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E113" t="s">
         <v>51</v>
@@ -8893,7 +8894,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2020</v>
       </c>
@@ -8901,10 +8902,10 @@
         <v>50</v>
       </c>
       <c r="C114" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D114" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E114" t="s">
         <v>51</v>
@@ -8946,7 +8947,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2020</v>
       </c>
@@ -8954,10 +8955,10 @@
         <v>50</v>
       </c>
       <c r="C115" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D115" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E115" t="s">
         <v>51</v>
@@ -8999,7 +9000,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -9046,7 +9047,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2020</v>
       </c>
@@ -9054,10 +9055,10 @@
         <v>322</v>
       </c>
       <c r="C117" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D117" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E117" t="s">
         <v>323</v>
@@ -9099,7 +9100,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2020</v>
       </c>
@@ -9107,7 +9108,7 @@
         <v>50</v>
       </c>
       <c r="C118" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D118" t="s">
         <v>779</v>
@@ -9152,7 +9153,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2020</v>
       </c>
@@ -9160,7 +9161,7 @@
         <v>524</v>
       </c>
       <c r="C119" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D119" t="s">
         <v>794</v>
@@ -9208,7 +9209,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2020</v>
       </c>
@@ -9216,7 +9217,7 @@
         <v>524</v>
       </c>
       <c r="C120" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D120" t="s">
         <v>794</v>
@@ -9264,7 +9265,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2020</v>
       </c>
@@ -9272,10 +9273,10 @@
         <v>550</v>
       </c>
       <c r="C121" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D121" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E121" t="s">
         <v>551</v>
@@ -9296,7 +9297,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2020</v>
       </c>
@@ -9304,10 +9305,10 @@
         <v>562</v>
       </c>
       <c r="C122" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D122" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E122" t="s">
         <v>563</v>
@@ -9328,7 +9329,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2020</v>
       </c>
@@ -9336,10 +9337,10 @@
         <v>587</v>
       </c>
       <c r="C123" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D123" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E123" t="s">
         <v>588</v>
@@ -9360,7 +9361,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2020</v>
       </c>
@@ -9392,7 +9393,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2020</v>
       </c>
@@ -9424,7 +9425,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2020</v>
       </c>
@@ -9432,10 +9433,10 @@
         <v>622</v>
       </c>
       <c r="C126" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D126" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E126" t="s">
         <v>623</v>
@@ -9456,7 +9457,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2020</v>
       </c>
@@ -9488,7 +9489,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2020</v>
       </c>
@@ -9496,10 +9497,10 @@
         <v>524</v>
       </c>
       <c r="C128" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D128" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E128" t="s">
         <v>692</v>
@@ -9520,7 +9521,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2020</v>
       </c>
@@ -9528,10 +9529,10 @@
         <v>711</v>
       </c>
       <c r="C129" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D129" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E129" t="s">
         <v>712</v>
@@ -9552,7 +9553,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2021</v>
       </c>
@@ -9560,10 +9561,10 @@
         <v>420</v>
       </c>
       <c r="C130" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D130" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E130" t="s">
         <v>421</v>
@@ -9614,7 +9615,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2021</v>
       </c>
@@ -9676,7 +9677,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2021</v>
       </c>
@@ -9684,10 +9685,10 @@
         <v>88</v>
       </c>
       <c r="C132" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D132" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E132" t="s">
         <v>89</v>
@@ -9723,7 +9724,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2021</v>
       </c>
@@ -9731,10 +9732,10 @@
         <v>151</v>
       </c>
       <c r="C133" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D133" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E133" t="s">
         <v>152</v>
@@ -9776,7 +9777,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2021</v>
       </c>
@@ -9835,7 +9836,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2021</v>
       </c>
@@ -9843,10 +9844,10 @@
         <v>279</v>
       </c>
       <c r="C135" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D135" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E135" t="s">
         <v>280</v>
@@ -9903,7 +9904,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2021</v>
       </c>
@@ -9911,7 +9912,7 @@
         <v>430</v>
       </c>
       <c r="C136" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D136" t="s">
         <v>779</v>
@@ -9956,7 +9957,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2021</v>
       </c>
@@ -10015,7 +10016,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2021</v>
       </c>
@@ -10023,10 +10024,10 @@
         <v>564</v>
       </c>
       <c r="C138" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D138" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E138" t="s">
         <v>565</v>
@@ -10047,7 +10048,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2021</v>
       </c>
@@ -10079,7 +10080,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2021</v>
       </c>
@@ -10087,10 +10088,10 @@
         <v>62</v>
       </c>
       <c r="C140" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D140" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E140" t="s">
         <v>63</v>
@@ -10145,7 +10146,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2021</v>
       </c>
@@ -10177,7 +10178,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2021</v>
       </c>
@@ -10209,7 +10210,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2021</v>
       </c>
@@ -10217,10 +10218,10 @@
         <v>668</v>
       </c>
       <c r="C143" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D143" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E143" t="s">
         <v>669</v>
@@ -10247,7 +10248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2022</v>
       </c>
@@ -10279,7 +10280,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2022</v>
       </c>
@@ -10287,10 +10288,10 @@
         <v>122</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D145" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E145" t="s">
         <v>123</v>
@@ -10332,7 +10333,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2022</v>
       </c>
@@ -10340,10 +10341,10 @@
         <v>426</v>
       </c>
       <c r="C146" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D146" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E146" t="s">
         <v>427</v>
@@ -10394,7 +10395,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2022</v>
       </c>
@@ -10402,10 +10403,10 @@
         <v>122</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D147" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E147" t="s">
         <v>123</v>
@@ -10447,7 +10448,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2022</v>
       </c>
@@ -10500,7 +10501,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2022</v>
       </c>
@@ -10508,10 +10509,10 @@
         <v>122</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D149" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E149" t="s">
         <v>123</v>
@@ -10553,7 +10554,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2022</v>
       </c>
@@ -10561,10 +10562,10 @@
         <v>122</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D150" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E150" t="s">
         <v>123</v>
@@ -10606,7 +10607,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2022</v>
       </c>
@@ -10614,10 +10615,10 @@
         <v>122</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D151" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E151" t="s">
         <v>123</v>
@@ -10659,7 +10660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2022</v>
       </c>
@@ -10667,10 +10668,10 @@
         <v>122</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D152" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E152" t="s">
         <v>123</v>
@@ -10712,7 +10713,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2022</v>
       </c>
@@ -10720,10 +10721,10 @@
         <v>122</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D153" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E153" t="s">
         <v>123</v>
@@ -10765,7 +10766,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2022</v>
       </c>
@@ -10773,10 +10774,10 @@
         <v>122</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D154" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E154" t="s">
         <v>123</v>
@@ -10818,7 +10819,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2022</v>
       </c>
@@ -10826,10 +10827,10 @@
         <v>122</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D155" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E155" t="s">
         <v>123</v>
@@ -10871,7 +10872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2022</v>
       </c>
@@ -10879,10 +10880,10 @@
         <v>122</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D156" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E156" t="s">
         <v>123</v>
@@ -10924,7 +10925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2022</v>
       </c>
@@ -10932,10 +10933,10 @@
         <v>122</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D157" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E157" t="s">
         <v>123</v>
@@ -10977,7 +10978,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2022</v>
       </c>
@@ -10985,10 +10986,10 @@
         <v>122</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D158" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E158" t="s">
         <v>123</v>
@@ -11030,7 +11031,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2022</v>
       </c>
@@ -11086,7 +11087,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2022</v>
       </c>
@@ -11148,7 +11149,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2022</v>
       </c>
@@ -11156,7 +11157,7 @@
         <v>731</v>
       </c>
       <c r="C161" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D161" t="s">
         <v>779</v>
@@ -11207,7 +11208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2022</v>
       </c>
@@ -11215,10 +11216,10 @@
         <v>122</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D162" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E162" t="s">
         <v>123</v>
@@ -11260,7 +11261,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2022</v>
       </c>
@@ -11305,7 +11306,7 @@
         <v>161</v>
       </c>
       <c r="O163" t="s">
-        <v>802</v>
+        <v>725</v>
       </c>
       <c r="P163" t="s">
         <v>131</v>
@@ -11320,7 +11321,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2022</v>
       </c>
@@ -11352,7 +11353,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2022</v>
       </c>
@@ -11360,7 +11361,7 @@
         <v>554</v>
       </c>
       <c r="C165" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D165" t="s">
         <v>779</v>
@@ -11384,7 +11385,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2022</v>
       </c>
@@ -11392,10 +11393,10 @@
         <v>556</v>
       </c>
       <c r="C166" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D166" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E166" t="s">
         <v>557</v>
@@ -11416,7 +11417,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2022</v>
       </c>
@@ -11424,10 +11425,10 @@
         <v>122</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D167" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E167" t="s">
         <v>123</v>
@@ -11469,7 +11470,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2022</v>
       </c>
@@ -11501,7 +11502,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2022</v>
       </c>
@@ -11509,10 +11510,10 @@
         <v>600</v>
       </c>
       <c r="C169" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D169" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E169" t="s">
         <v>601</v>
@@ -11533,7 +11534,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2022</v>
       </c>
@@ -11565,7 +11566,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2022</v>
       </c>
@@ -11573,10 +11574,10 @@
         <v>596</v>
       </c>
       <c r="C171" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D171" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E171" t="s">
         <v>597</v>
@@ -11597,7 +11598,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2022</v>
       </c>
@@ -11629,7 +11630,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2022</v>
       </c>
@@ -11661,7 +11662,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2022</v>
       </c>
@@ -11669,10 +11670,10 @@
         <v>630</v>
       </c>
       <c r="C174" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D174" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E174" t="s">
         <v>631</v>
@@ -11693,7 +11694,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2022</v>
       </c>
@@ -11725,7 +11726,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2022</v>
       </c>
@@ -11733,7 +11734,7 @@
         <v>683</v>
       </c>
       <c r="C176" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D176" t="s">
         <v>779</v>
@@ -11808,9 +11809,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>719</v>
       </c>

</xml_diff>